<commit_message>
Final cleanup and push of completed project.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/GiftCardData.xlsx
+++ b/src/test/resources/data/GiftCardData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>TestCases</t>
   </si>
@@ -149,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -164,6 +164,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
@@ -514,7 +523,7 @@
       <c r="F2" s="6">
         <v>9087654321</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -537,7 +546,7 @@
       <c r="F3" s="6">
         <v>67436778</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="27" t="s">
         <v>15</v>
       </c>
     </row>
@@ -560,7 +569,7 @@
       <c r="F4" s="6">
         <v>9087654321</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="28" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>